<commit_message>
Completd employee bulk upload
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template-v2.xlsx
+++ b/upload/template/employee/Bulk Upload Template-v2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -99,16 +99,13 @@
     <t xml:space="preserve">E0132</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrunali Desai</t>
+    <t xml:space="preserve">Mruali Desai</t>
   </si>
   <si>
     <t xml:space="preserve">Java Developer</t>
   </si>
   <si>
     <t xml:space="preserve">desaimrunali777@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0133</t>
   </si>
   <si>
     <t xml:space="preserve">Vinit Dhondapati</t>
@@ -426,7 +423,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -509,7 +506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
@@ -546,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>44920</v>
@@ -558,13 +555,13 @@
         <v>35952</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="I4" s="9" t="n">
         <v>1234543267</v>
@@ -618,10 +615,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +650,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete bulk upload for role and technology
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template-v2.xlsx
+++ b/upload/template/employee/Bulk Upload Template-v2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t xml:space="preserve">E0131</t>
+    <t xml:space="preserve">E0133</t>
   </si>
   <si>
     <t xml:space="preserve">Ranjana Mishra</t>
@@ -87,37 +87,13 @@
     <t xml:space="preserve">Solution Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">mishranjana21@gmail.com</t>
+    <t xml:space="preserve">shonamishra170@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
   </si>
   <si>
     <t xml:space="preserve">Pune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mruali Desai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java Developer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">desaimrunali777@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vinit Dhondapati</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dondapativinit@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -309,8 +285,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="A1:K4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table3" displayName="Table3" ref="A1:K2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K2"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Sr No"/>
     <tableColumn id="2" name="EMP ID"/>
@@ -420,10 +396,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,81 +482,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>44919</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>36657</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <v>9876452367</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>44920</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>35952</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="9" t="n">
-        <v>1234543267</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="mishranjana21@gmail.com"/>
-    <hyperlink ref="G3" r:id="rId2" display="desaimrunali777@gmail.com"/>
-    <hyperlink ref="G4" r:id="rId3" display="dondapativinit@gmail.com"/>
+    <hyperlink ref="G2" r:id="rId1" display="shonamishra170@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -590,7 +502,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -615,10 +527,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs in employee bulk upload
</commit_message>
<xml_diff>
--- a/upload/template/employee/Bulk Upload Template-v2.xlsx
+++ b/upload/template/employee/Bulk Upload Template-v2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t xml:space="preserve">Sr. No</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t xml:space="preserve">Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E0134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pratiksha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pratiksha1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Sr.No</t>
@@ -399,7 +414,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -482,9 +497,102 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="9" t="n">
+        <v>8723456712</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="9" t="n">
+        <v>8723456712</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>44918</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>35952</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="9" t="n">
+        <v>8723456712</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -493,6 +601,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="shonamishra170@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="shonamishra170@gmail.com"/>
+    <hyperlink ref="G4" r:id="rId3" display="p1@gmail.com"/>
+    <hyperlink ref="G5" r:id="rId4" display="p2@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -502,7 +613,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -527,10 +638,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +673,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,7 +681,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>